<commit_message>
making session/cookie for autologin
</commit_message>
<xml_diff>
--- a/myHome 개발일지.xlsx
+++ b/myHome 개발일지.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="작업진행" sheetId="1" r:id="rId1"/>
-    <sheet name="목표" sheetId="2" r:id="rId2"/>
+    <sheet name="ToDo List" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">목표!$A$1:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ToDo List'!$A$1:$B$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">작업진행!$A$1:$F$7</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>작업내용</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -203,10 +203,6 @@
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -306,16 +302,77 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>진행</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>linux.js
 linix.ejs</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>리눅스/로그 관련 기능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>즐겨찾기 관리 기능 같은 메뉴 커스텀 기능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.ejs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초기설정 페이지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인설정 관리 페이지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>붙여넣기/잘라내기 하고 나면 폴더 이동 에러 &gt;&gt; 폴더 이름이 "download/" 같은 형식이면, /로 split 하므로 문제가 생겼음 &gt;&gt; fullname에서 끝자리가 /일 경우를 처리하는 로직을 추가
+체크박스 전체 체크/전체 해제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.js에서 /control을 분리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/routes/control.js로 분리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메뉴 커스텀 기능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>체크한 목록 확인을 클로저로 분리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠키와 세션을 이용한 자동로그인 기능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sqlite</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>npm으로 sqlite3 설치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션과 mysql 연동 해제</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -725,13 +782,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -829,7 +886,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>24</v>
@@ -846,10 +903,10 @@
         <v>43773</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
@@ -863,27 +920,109 @@
         <v>43773</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3">
         <v>43773</v>
       </c>
+      <c r="C8" s="3">
+        <v>43773</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43773</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43773</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3">
+        <v>43773</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43773</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3">
+        <v>43773</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43773</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43773</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43773</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -897,11 +1036,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -965,28 +1104,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -997,8 +1136,32 @@
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B9">
+  <autoFilter ref="A1:B14">
     <filterColumn colId="0">
       <filters>
         <filter val="N"/>

</xml_diff>